<commit_message>
make mapper handle empty columns properly and added test for it
</commit_message>
<xml_diff>
--- a/easybatch-extensions/easybatch-msexcel/src/test/resources/tweets-in.xlsx
+++ b/easybatch-extensions/easybatch-msexcel/src/test/resources/tweets-in.xlsx
@@ -1,17 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan.atanasov/Code/easy-batch/easybatch-extensions/easybatch-msexcel/src/test/resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
+    <workbookView xWindow="-19320" yWindow="-23540" windowWidth="38400" windowHeight="23540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -122,12 +135,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -157,12 +170,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -369,12 +382,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1">
         <v>1</v>
       </c>
@@ -385,7 +398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -407,7 +420,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -419,7 +432,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
revert javadoc and input excel file
</commit_message>
<xml_diff>
--- a/easybatch-extensions/easybatch-msexcel/src/test/resources/tweets-in.xlsx
+++ b/easybatch-extensions/easybatch-msexcel/src/test/resources/tweets-in.xlsx
@@ -1,30 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28502"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan.atanasov/Code/easy-batch/easybatch-extensions/easybatch-msexcel/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-23540" windowWidth="38400" windowHeight="23540"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -135,12 +122,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -170,12 +157,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -382,12 +369,12 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
@@ -398,7 +385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
@@ -420,7 +407,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -432,7 +419,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>